<commit_message>
add processed data for geo, tar pod5 files
</commit_message>
<xml_diff>
--- a/metadata/SRA_seq_template.xlsx
+++ b/metadata/SRA_seq_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurakwhite/Library/CloudStorage/Dropbox/Laura - UC Denver/2023/tRNAworkshop/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04FCAD56-9715-B64D-9A44-9C8DFD739EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD17998-60DF-B74B-AE81-DF623FBA852A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30580" yWindow="500" windowWidth="39840" windowHeight="24320" xr2:uid="{E323A56D-B1B0-694F-9793-7AFEC17DEDAF}"/>
+    <workbookView xWindow="30580" yWindow="500" windowWidth="45860" windowHeight="25840" xr2:uid="{E323A56D-B1B0-694F-9793-7AFEC17DEDAF}"/>
   </bookViews>
   <sheets>
     <sheet name="2. Metadata Template " sheetId="2" r:id="rId1"/>
@@ -3832,7 +3832,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="187">
   <si>
     <r>
       <rPr>
@@ -4300,51 +4300,27 @@
     <t>T. thermophila RNA004 chemistry</t>
   </si>
   <si>
-    <t>Drosophila002_20231207_1500_MN35252_FAX30455_48242de2.pod5.gz</t>
-  </si>
-  <si>
     <t>Drosophila002_20231207_1500_MN35252_FAX30455_48242de2.rna002_70bps_hac@v3.fastq.gz</t>
   </si>
   <si>
-    <t>Drosophila004_20231208_1307_MN31004_FAX73799_72c200e4.pod5.gz</t>
-  </si>
-  <si>
     <t>Drosophila004_20231208_1307_MN31004_FAX73799_72c200e4.rna004_130bps_sup@v5.0.0.fastq.gz</t>
   </si>
   <si>
-    <t>Ecoli002_20231208_1312_P2S-00519-A_PAS44628_9e5214a7.pod5.gz</t>
-  </si>
-  <si>
     <t>Ecoli002_20231208_1312_P2S-00519-A_PAS44628_9e5214a7.rna002_70bps_hac@v3.fastq.gz</t>
   </si>
   <si>
-    <t>Ecoli004_20240105_1224_MN31004_FAX73799_1fe84761.pod5.gz</t>
-  </si>
-  <si>
     <t>Ecoli004_20240105_1224_MN31004_FAX73799_1fe84761.rna004_130bps_sup@v5.0.0.fastq.gz</t>
   </si>
   <si>
-    <t>Grandeyeast004_20240105_1222_P2S-00519-B_PAS98845_231d7d7e.pod5.gz</t>
-  </si>
-  <si>
     <t>Grandeyeast004_20240105_1222_P2S-00519-B_PAS98845_231d7d7e.rna004_130bps_sup@v5.0.0.fastq.gz</t>
   </si>
   <si>
-    <t>HumanFibroblast002_20231207_1455_P2S-00519-B_PAS29437_b7f6c4bd.pod5.gz</t>
-  </si>
-  <si>
     <t>HumanFibroblast002_20231207_1455_P2S-00519-B_PAS29437_b7f6c4bd.rna002_70bps_hac@v3.fastq.gz</t>
   </si>
   <si>
-    <t>HumanFibroblast004_20231208_1351_MN42516_FAX71838_b8f7b990.pod5.gz</t>
-  </si>
-  <si>
     <t>HumanFibroblast004_20231208_1351_MN42516_FAX71838_b8f7b990.rna004_130bps_sup@v5.0.0.fastq.gz</t>
   </si>
   <si>
-    <t>Petityeast004_20240105_1222_P2S-00519-A_PAQ47538_49891fce.pod5.gz</t>
-  </si>
-  <si>
     <t>Petityeast004_20240105_1222_P2S-00519-A_PAQ47538_49891fce.rna004_130bps_sup@v5.0.0.fastq.gz</t>
   </si>
   <si>
@@ -4354,24 +4330,12 @@
     <t>Zebrafish002_20231207_1528_P2S-00519-A_PAS44221_7e583c4c.rna002_70bps_hac@v3.fastq.gz</t>
   </si>
   <si>
-    <t>Zebrafish002_20231207_1528_P2S-00519-A_PAS44221_7e583c4c.pod5.gz</t>
-  </si>
-  <si>
-    <t>Zebrafish004_20231208_0919_MN31004_FAX73799_f3dea9f8.pod5.gz</t>
-  </si>
-  <si>
     <t>Zebrafish004_20231208_0919_MN31004_FAX73799_f3dea9f8.rna004_130bps_sup@v5.0.0.fastq.gz</t>
   </si>
   <si>
     <t>Tetrahymena002_20231207_1743_MN35252_FAX30455_c9f80979.rna002_70bps_hac@v3.fastq.gz</t>
   </si>
   <si>
-    <t>Tetrahymena002_20231207_1743_MN35252_FAX30455_c9f80979.pod5.gz</t>
-  </si>
-  <si>
-    <t>Tetrahymena004_20231208_0920_MN42516_FAX71838_a244513d.pod5.gz</t>
-  </si>
-  <si>
     <t>Tetrahymena004_20231208_0920_MN42516_FAX71838_a244513d.rna004_130bps_sup@v5.0.0.fastq.gz</t>
   </si>
   <si>
@@ -4381,15 +4345,9 @@
     <t>WTyeast004_20231111_1104_P2S-00519-B_PAQ47538_fa3726ec.rna004_130bps_sup@v5.0.0.fastq.gz</t>
   </si>
   <si>
-    <t>Pus1yeast004_20240105_1330_P2S-00519-A_PAS92267_56de71b8.pod5.gz</t>
-  </si>
-  <si>
     <t>Pus1yeast004_20240105_1330_P2S-00519-A_PAS92267_56de71b8.rna004_130bps_sup@v5.0.0.fastq.gz</t>
   </si>
   <si>
-    <t>Pus2yeast004_20240105_1330_P2S-00519-B_PAS98920_19ba906c.pod5.gz</t>
-  </si>
-  <si>
     <t>Pus2yeast004_20240105_1330_P2S-00519-B_PAS98920_19ba906c.rna004_130bps_sup@v5.0.0.fastq.gz</t>
   </si>
   <si>
@@ -4399,24 +4357,9 @@
     <t>Pus4yeast004_20231208_1152_MN42516_FAX71838_e2d70aac.rna004_130bps_sup@v5.0.0.fastq.gz</t>
   </si>
   <si>
-    <t>Pus4yeast004_20231208_1152_MN42516_FAX71838_e2d70aac.pod5.gz</t>
-  </si>
-  <si>
-    <t>Pus4yeast002_20231208_1601_MN31004_FAX30455_c72fd68f.pod5.gz</t>
-  </si>
-  <si>
     <t>T4phage004_20240202_1332_P2S-01618-A_PAU05281_fd3805fc.rna004_130bps_sup@v5.0.0.fastq.gz</t>
   </si>
   <si>
-    <t>WTyeast002_20231111_1103_P2S-00519-A_PAS43478_1fa49e43.pod5.gz</t>
-  </si>
-  <si>
-    <t>WTyeast004_20231111_1104_P2S-00519-B_PAQ47538_fa3726ec.pod5.gz</t>
-  </si>
-  <si>
-    <t>T4phage004_20240202_1332_P2S-01618-A_PAU05281_fd3805fc.pod5.gz</t>
-  </si>
-  <si>
     <t>Comparative analysis of 43 distinct RNA modifications by nanopore tRNA sequencing</t>
   </si>
   <si>
@@ -4475,13 +4418,130 @@
   </si>
   <si>
     <t>MG1655</t>
+  </si>
+  <si>
+    <t>Zebrafish002_20231207_1528_P2S-00519-A_PAS44221_7e583c4c.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>Zebrafish004_20231208_0919_MN31004_FAX73799_f3dea9f8.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>Drosophila002_20231207_1500_MN35252_FAX30455_48242de2.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>Drosophila004_20231208_1307_MN31004_FAX73799_72c200e4.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>Ecoli002_20231208_1312_P2S-00519-A_PAS44628_9e5214a7.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>Ecoli004_20240105_1224_MN31004_FAX73799_1fe84761.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>T4phage004_20240202_1332_P2S-01618-A_PAU05281_fd3805fc.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>HumanFibroblast002_20231207_1455_P2S-00519-B_PAS29437_b7f6c4bd.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>HumanFibroblast004_20231208_1351_MN42516_FAX71838_b8f7b990.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>Grandeyeast004_20240105_1222_P2S-00519-B_PAS98845_231d7d7e.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>Petityeast004_20240105_1222_P2S-00519-A_PAQ47538_49891fce.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>Pus1yeast004_20240105_1330_P2S-00519-A_PAS92267_56de71b8.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>Pus2yeast004_20240105_1330_P2S-00519-B_PAS98920_19ba906c.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>Pus4yeast002_20231208_1601_MN31004_FAX30455_c72fd68f.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>Pus4yeast004_20231208_1152_MN42516_FAX71838_e2d70aac.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>WTyeast002_20231111_1103_P2S-00519-A_PAS43478_1fa49e43.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>WTyeast004_20231111_1104_P2S-00519-B_PAQ47538_fa3726ec.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>Tetrahymena002_20231207_1743_MN35252_FAX30455_c9f80979.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>Tetrahymena004_20231208_0920_MN42516_FAX71838_a244513d.pod5.tar.gz</t>
+  </si>
+  <si>
+    <t>Zebrafish002_20231207_1528_P2S-00519-A_PAS44221_7e583c4c.rna002_70bps_hac@v3.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>Zebrafish004_20231208_0919_MN31004_FAX73799_f3dea9f8.rna004_130bps_sup@v5.0.0.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>Drosophila002_20231207_1500_MN35252_FAX30455_48242de2.rna002_70bps_hac@v3.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>Drosophila004_20231208_1307_MN31004_FAX73799_72c200e4.rna004_130bps_sup@v5.0.0.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>Ecoli002_20231208_1312_P2S-00519-A_PAS44628_9e5214a7.rna002_70bps_hac@v3.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>Ecoli004_20240105_1224_MN31004_FAX73799_1fe84761.rna004_130bps_sup@v5.0.0.T4ref.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>Ecoli004_20240105_1224_MN31004_FAX73799_1fe84761.rna004_130bps_sup@v5.0.0.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>Grandeyeast004_20240105_1222_P2S-00519-B_PAS98845_231d7d7e.rna004_130bps_sup@v5.0.0.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>HumanFibroblast002_20231207_1455_P2S-00519-B_PAS29437_b7f6c4bd.rna002_70bps_hac@v3.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>HumanFibroblast004_20231208_1351_MN42516_FAX71838_b8f7b990.rna004_130bps_sup@v5.0.0.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>Petityeast004_20240105_1222_P2S-00519-A_PAQ47538_49891fce.rna004_130bps_sup@v5.0.0.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>Pus1yeast004_20240105_1330_P2S-00519-A_PAS92267_56de71b8.rna004_130bps_sup@v5.0.0.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>Pus2yeast004_20240105_1330_P2S-00519-B_PAS98920_19ba906c.rna004_130bps_sup@v5.0.0.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>Pus4yeast002_20231208_1601_MN31004_FAX30455_c72fd68f.rna002_70bps_hac@v3.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>T4infectedecoli_20240202_1332_P2S-01618-A_PAU05281_fd3805fc.rna004_130bps_sup@v5.0.0.T4ref.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>Tetrahymena002_20231207_1743_MN35252_FAX30455_c9f80979.rna002_70bps_hac@v3.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>Tetrahymena004_20231208_0920_MN42516_FAX71838_a244513d.rna004_130bps_sup@v5.0.0.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>WTyeast002_20231111_1103_P2S-00519-A_PAS43478_1fa49e43.rna002_70bps_hac@v3.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>WTyeast004_20231111_1104_P2S-00519-B_PAQ47538_fa3726ec.rna004_130bps_sup@v5.0.0.bwa_full_length.bam.fl.bg</t>
+  </si>
+  <si>
+    <t>Pus4yeast004_20231208_1601_MN31004_FAX30455_c72fd68f.rna002_130bps_sup@v5.0.0.bwa_full_length.bam.fl.bg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4616,6 +4676,11 @@
       <color rgb="FF434343"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Inconsolata"/>
     </font>
   </fonts>
   <fills count="7">
@@ -4784,12 +4849,10 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -5598,11 +5661,11 @@
   </sheetPr>
   <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:XFD57"/>
+    <sheetView tabSelected="1" topLeftCell="I10" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="83.6640625" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="83.6640625" defaultRowHeight="14" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="29.83203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" style="6" customWidth="1"/>
@@ -5616,19 +5679,20 @@
     <col min="10" max="10" width="7.6640625" style="6" customWidth="1"/>
     <col min="11" max="11" width="11.5" style="6" customWidth="1"/>
     <col min="12" max="12" width="23" style="6" customWidth="1"/>
-    <col min="13" max="14" width="10" style="6" customWidth="1"/>
+    <col min="13" max="13" width="68" style="6" customWidth="1"/>
+    <col min="14" max="14" width="10" style="6" customWidth="1"/>
     <col min="15" max="15" width="66.6640625" style="6" customWidth="1"/>
     <col min="16" max="16" width="71.83203125" style="6" customWidth="1"/>
     <col min="17" max="18" width="20" style="6" customWidth="1"/>
     <col min="19" max="16384" width="83.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="14" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" s="3" customFormat="1" ht="14" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -5637,21 +5701,21 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:16" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" s="5" customFormat="1" ht="14" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:16" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="5" customFormat="1" ht="14" customHeight="1">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="6" spans="1:16" s="9" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="9" customFormat="1" ht="14" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -5671,7 +5735,7 @@
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
     </row>
-    <row r="7" spans="1:16" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" s="12" customFormat="1" ht="14" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
@@ -5691,7 +5755,7 @@
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" s="12" customFormat="1" ht="14" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
@@ -5710,159 +5774,159 @@
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="14" customHeight="1">
       <c r="A9" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="14" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="14" customHeight="1">
       <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="14" customHeight="1">
       <c r="A12" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="14" customHeight="1">
       <c r="A13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="35" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="14" customHeight="1">
       <c r="A14" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="35" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="34" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="14" customHeight="1">
       <c r="A15" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="35" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="34" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="14" customHeight="1">
       <c r="A16" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="35" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="34" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="14" customHeight="1">
       <c r="A17" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="35" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="34" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="14" customHeight="1">
       <c r="A18" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="35" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="14" customHeight="1">
       <c r="A19" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="35" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="34" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="14" customHeight="1">
       <c r="A20" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="35" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="14" customHeight="1">
       <c r="A21" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="35" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="14" customHeight="1">
       <c r="A22" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="35" t="s">
-        <v>160</v>
+      <c r="B22" s="34" t="s">
+        <v>141</v>
       </c>
       <c r="D22" s="15"/>
     </row>
-    <row r="23" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:16" ht="14" customHeight="1">
       <c r="A23" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="35" t="s">
-        <v>161</v>
+      <c r="B23" s="34" t="s">
+        <v>142</v>
       </c>
       <c r="D23" s="15"/>
     </row>
-    <row r="24" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:16" ht="14" customHeight="1">
       <c r="A24" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="35" t="s">
-        <v>162</v>
+      <c r="B24" s="34" t="s">
+        <v>143</v>
       </c>
       <c r="D24" s="15"/>
     </row>
-    <row r="25" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:16" ht="14" customHeight="1">
       <c r="A25" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="35"/>
-    </row>
-    <row r="26" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="34"/>
+    </row>
+    <row r="26" spans="1:16" ht="14" customHeight="1">
       <c r="A26" s="16"/>
     </row>
-    <row r="27" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="14" customHeight="1">
       <c r="A27" s="16"/>
     </row>
-    <row r="28" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="14" customHeight="1">
       <c r="A28" s="16"/>
     </row>
-    <row r="29" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="14" customHeight="1">
       <c r="A29" s="16"/>
     </row>
-    <row r="30" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="14" customHeight="1">
       <c r="A30" s="16"/>
     </row>
-    <row r="31" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="14" customHeight="1">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -5880,7 +5944,7 @@
       <c r="O31" s="17"/>
       <c r="P31" s="17"/>
     </row>
-    <row r="32" spans="1:16" s="9" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" s="9" customFormat="1" ht="14" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>10</v>
       </c>
@@ -5900,7 +5964,7 @@
       <c r="O32" s="7"/>
       <c r="P32" s="8"/>
     </row>
-    <row r="33" spans="1:18" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" s="12" customFormat="1" ht="14" customHeight="1">
       <c r="A33" s="10" t="s">
         <v>11</v>
       </c>
@@ -5920,7 +5984,7 @@
       <c r="O33" s="10"/>
       <c r="P33" s="11"/>
     </row>
-    <row r="34" spans="1:18" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" s="12" customFormat="1" ht="14" customHeight="1">
       <c r="A34" s="10" t="s">
         <v>12</v>
       </c>
@@ -5940,7 +6004,7 @@
       <c r="O34" s="10"/>
       <c r="P34" s="11"/>
     </row>
-    <row r="35" spans="1:18" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" s="20" customFormat="1" ht="14" customHeight="1">
       <c r="A35" s="18" t="s">
         <v>13</v>
       </c>
@@ -5960,7 +6024,7 @@
       <c r="O35" s="18"/>
       <c r="P35" s="19"/>
     </row>
-    <row r="36" spans="1:18" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" s="20" customFormat="1" ht="14" customHeight="1">
       <c r="A36" s="18" t="s">
         <v>14</v>
       </c>
@@ -5980,7 +6044,7 @@
       <c r="O36" s="18"/>
       <c r="P36" s="19"/>
     </row>
-    <row r="37" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" ht="14" customHeight="1">
       <c r="A37" s="21" t="s">
         <v>15</v>
       </c>
@@ -6036,22 +6100,22 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:18" ht="14" customHeight="1">
       <c r="A38" s="24" t="s">
         <v>69</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C38" s="34" t="s">
+      <c r="C38" s="33" t="s">
         <v>54</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="E38" s="26"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
       <c r="I38" s="26" t="s">
         <v>47</v>
       </c>
@@ -6059,36 +6123,38 @@
         <v>46</v>
       </c>
       <c r="K38" s="25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L38" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="M38" s="25"/>
+      <c r="M38" s="36" t="s">
+        <v>167</v>
+      </c>
       <c r="N38" s="25"/>
       <c r="O38" s="6" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="14" customHeight="1">
       <c r="A39" s="24" t="s">
         <v>70</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="33" t="s">
         <v>54</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="E39" s="26"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
       <c r="I39" s="26" t="s">
         <v>47</v>
       </c>
@@ -6101,23 +6167,25 @@
       <c r="L39" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="M39" s="25"/>
+      <c r="M39" s="36" t="s">
+        <v>168</v>
+      </c>
       <c r="N39" s="25"/>
       <c r="O39" s="6" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="P39" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="14" customHeight="1">
       <c r="A40" s="24" t="s">
         <v>71</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="34" t="s">
+      <c r="C40" s="33" t="s">
         <v>55</v>
       </c>
       <c r="D40" s="25"/>
@@ -6125,7 +6193,7 @@
         <v>60</v>
       </c>
       <c r="F40" s="26"/>
-      <c r="H40" s="33"/>
+      <c r="H40" s="26"/>
       <c r="I40" s="26" t="s">
         <v>47</v>
       </c>
@@ -6138,23 +6206,25 @@
       <c r="L40" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="M40" s="25"/>
+      <c r="M40" s="36" t="s">
+        <v>169</v>
+      </c>
       <c r="N40" s="25"/>
       <c r="O40" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="14" customHeight="1">
       <c r="A41" s="24" t="s">
         <v>72</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="33" t="s">
         <v>55</v>
       </c>
       <c r="D41" s="25"/>
@@ -6162,8 +6232,8 @@
         <v>60</v>
       </c>
       <c r="F41" s="26"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
       <c r="I41" s="26" t="s">
         <v>47</v>
       </c>
@@ -6176,32 +6246,34 @@
       <c r="L41" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="M41" s="25"/>
+      <c r="M41" s="36" t="s">
+        <v>170</v>
+      </c>
       <c r="N41" s="25"/>
       <c r="O41" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P41" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="14" customHeight="1">
       <c r="A42" s="24" t="s">
         <v>73</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="34" t="s">
+      <c r="C42" s="33" t="s">
         <v>56</v>
       </c>
       <c r="D42" s="25"/>
       <c r="E42" s="26" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="F42" s="26"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="33"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
       <c r="I42" s="26" t="s">
         <v>47</v>
       </c>
@@ -6209,37 +6281,39 @@
         <v>46</v>
       </c>
       <c r="K42" s="25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L42" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="M42" s="25"/>
+      <c r="M42" s="36" t="s">
+        <v>171</v>
+      </c>
       <c r="N42" s="25"/>
       <c r="O42" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="P42" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="14" customHeight="1">
       <c r="A43" s="24" t="s">
         <v>74</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C43" s="34" t="s">
+      <c r="C43" s="33" t="s">
         <v>56</v>
       </c>
       <c r="D43" s="25"/>
       <c r="E43" s="26" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="F43" s="26"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
       <c r="I43" s="26" t="s">
         <v>47</v>
       </c>
@@ -6252,28 +6326,32 @@
       <c r="L43" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="M43" s="25"/>
-      <c r="N43" s="25"/>
+      <c r="M43" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="N43" s="36" t="s">
+        <v>173</v>
+      </c>
       <c r="O43" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="P43" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="14" customHeight="1">
       <c r="A44" s="24" t="s">
         <v>75</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="33" t="s">
         <v>56</v>
       </c>
       <c r="D44" s="25"/>
       <c r="E44" s="26" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
@@ -6286,32 +6364,36 @@
       <c r="J44" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K44" s="25"/>
+      <c r="K44" s="25" t="s">
+        <v>116</v>
+      </c>
       <c r="L44" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="M44" s="25"/>
+      <c r="M44" s="36" t="s">
+        <v>181</v>
+      </c>
       <c r="N44" s="25"/>
       <c r="O44" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="P44" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="14" customHeight="1">
       <c r="A45" s="24" t="s">
         <v>76</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="34" t="s">
+      <c r="C45" s="33" t="s">
         <v>57</v>
       </c>
       <c r="D45" s="25"/>
-      <c r="E45" s="36" t="s">
-        <v>164</v>
+      <c r="E45" s="35" t="s">
+        <v>145</v>
       </c>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
@@ -6323,33 +6405,35 @@
         <v>46</v>
       </c>
       <c r="K45" s="25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L45" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="M45" s="25"/>
+      <c r="M45" s="36" t="s">
+        <v>175</v>
+      </c>
       <c r="N45" s="25"/>
       <c r="O45" s="6" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="P45" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="14" customHeight="1">
       <c r="A46" s="24" t="s">
         <v>77</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="34" t="s">
+      <c r="C46" s="33" t="s">
         <v>57</v>
       </c>
       <c r="D46" s="25"/>
-      <c r="E46" s="36" t="s">
-        <v>164</v>
+      <c r="E46" s="35" t="s">
+        <v>145</v>
       </c>
       <c r="F46" s="26"/>
       <c r="G46" s="26"/>
@@ -6366,23 +6450,25 @@
       <c r="L46" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="M46" s="25"/>
+      <c r="M46" s="36" t="s">
+        <v>176</v>
+      </c>
       <c r="N46" s="25"/>
       <c r="O46" s="6" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="P46" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="14" customHeight="1">
       <c r="A47" s="24" t="s">
         <v>78</v>
       </c>
       <c r="B47" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="C47" s="33" t="s">
         <v>58</v>
       </c>
       <c r="D47" s="25"/>
@@ -6401,28 +6487,30 @@
         <v>46</v>
       </c>
       <c r="K47" s="25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L47" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="M47" s="25"/>
+      <c r="M47" s="36" t="s">
+        <v>174</v>
+      </c>
       <c r="N47" s="25"/>
       <c r="O47" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="P47" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="14" customHeight="1">
       <c r="A48" s="24" t="s">
         <v>79</v>
       </c>
       <c r="B48" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C48" s="33" t="s">
         <v>58</v>
       </c>
       <c r="D48" s="25"/>
@@ -6441,28 +6529,30 @@
         <v>46</v>
       </c>
       <c r="K48" s="25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L48" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="M48" s="25"/>
+      <c r="M48" s="36" t="s">
+        <v>177</v>
+      </c>
       <c r="N48" s="25"/>
       <c r="O48" s="6" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="P48" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="14" customHeight="1">
       <c r="A49" s="24" t="s">
         <v>80</v>
       </c>
       <c r="B49" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="C49" s="34" t="s">
+      <c r="C49" s="33" t="s">
         <v>58</v>
       </c>
       <c r="D49" s="25"/>
@@ -6481,28 +6571,30 @@
         <v>46</v>
       </c>
       <c r="K49" s="25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L49" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="M49" s="25"/>
+      <c r="M49" s="36" t="s">
+        <v>178</v>
+      </c>
       <c r="N49" s="25"/>
       <c r="O49" s="6" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="P49" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="14" customHeight="1">
       <c r="A50" s="24" t="s">
         <v>81</v>
       </c>
       <c r="B50" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="C50" s="34" t="s">
+      <c r="C50" s="33" t="s">
         <v>58</v>
       </c>
       <c r="D50" s="25"/>
@@ -6521,28 +6613,30 @@
         <v>46</v>
       </c>
       <c r="K50" s="25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L50" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="M50" s="25"/>
+      <c r="M50" s="36" t="s">
+        <v>179</v>
+      </c>
       <c r="N50" s="25"/>
       <c r="O50" s="6" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="P50" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="14" customHeight="1">
       <c r="A51" s="24" t="s">
         <v>82</v>
       </c>
       <c r="B51" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="C51" s="34" t="s">
+      <c r="C51" s="33" t="s">
         <v>58</v>
       </c>
       <c r="D51" s="25"/>
@@ -6566,23 +6660,25 @@
       <c r="L51" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="M51" s="25"/>
+      <c r="M51" s="36" t="s">
+        <v>180</v>
+      </c>
       <c r="N51" s="25"/>
       <c r="O51" s="6" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="P51" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="14" customHeight="1">
       <c r="A52" s="24" t="s">
         <v>83</v>
       </c>
       <c r="B52" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="34" t="s">
+      <c r="C52" s="33" t="s">
         <v>58</v>
       </c>
       <c r="D52" s="25"/>
@@ -6606,23 +6702,25 @@
       <c r="L52" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="M52" s="25"/>
+      <c r="M52" s="36" t="s">
+        <v>186</v>
+      </c>
       <c r="N52" s="25"/>
       <c r="O52" s="6" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="P52" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="14" customHeight="1">
       <c r="A53" s="24" t="s">
         <v>85</v>
       </c>
       <c r="B53" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="C53" s="34" t="s">
+      <c r="C53" s="33" t="s">
         <v>58</v>
       </c>
       <c r="D53" s="25"/>
@@ -6641,28 +6739,30 @@
         <v>46</v>
       </c>
       <c r="K53" s="25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L53" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="M53" s="25"/>
+      <c r="M53" s="36" t="s">
+        <v>184</v>
+      </c>
       <c r="N53" s="25"/>
       <c r="O53" s="6" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="P53" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="14" customHeight="1">
       <c r="A54" s="24" t="s">
         <v>84</v>
       </c>
       <c r="B54" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="C54" s="34" t="s">
+      <c r="C54" s="33" t="s">
         <v>58</v>
       </c>
       <c r="D54" s="25"/>
@@ -6681,28 +6781,30 @@
         <v>46</v>
       </c>
       <c r="K54" s="25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L54" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="M54" s="25"/>
+      <c r="M54" s="36" t="s">
+        <v>185</v>
+      </c>
       <c r="N54" s="25"/>
       <c r="O54" s="6" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="P54" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="14" customHeight="1">
       <c r="A55" s="24" t="s">
         <v>86</v>
       </c>
       <c r="B55" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="34" t="s">
+      <c r="C55" s="33" t="s">
         <v>59</v>
       </c>
       <c r="D55" s="25"/>
@@ -6722,22 +6824,24 @@
       <c r="L55" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="M55" s="25"/>
+      <c r="M55" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="O55" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="P55" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="14" customHeight="1">
       <c r="A56" s="24" t="s">
         <v>87</v>
       </c>
       <c r="B56" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="34" t="s">
+      <c r="C56" s="33" t="s">
         <v>59</v>
       </c>
       <c r="D56" s="25"/>
@@ -6757,15 +6861,17 @@
       <c r="L56" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="M56" s="25"/>
+      <c r="M56" s="36" t="s">
+        <v>183</v>
+      </c>
       <c r="O56" s="6" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="P56" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" s="9" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" s="9" customFormat="1" ht="14" customHeight="1">
       <c r="A57" s="3" t="s">
         <v>28</v>
       </c>
@@ -6785,7 +6891,7 @@
       <c r="O57" s="7"/>
       <c r="P57" s="8"/>
     </row>
-    <row r="58" spans="1:16" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" s="12" customFormat="1" ht="14" customHeight="1">
       <c r="A58" s="10" t="s">
         <v>29</v>
       </c>
@@ -6805,7 +6911,7 @@
       <c r="O58" s="10"/>
       <c r="P58" s="11"/>
     </row>
-    <row r="59" spans="1:16" s="29" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" s="29" customFormat="1" ht="14" customHeight="1">
       <c r="A59" s="27" t="s">
         <v>30</v>
       </c>
@@ -6825,7 +6931,7 @@
       <c r="O59" s="27"/>
       <c r="P59" s="28"/>
     </row>
-    <row r="60" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" ht="14" customHeight="1">
       <c r="A60" s="13" t="s">
         <v>31</v>
       </c>
@@ -6845,7 +6951,7 @@
       <c r="O60" s="25"/>
       <c r="P60" s="25"/>
     </row>
-    <row r="61" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" ht="14" customHeight="1">
       <c r="A61" s="13" t="s">
         <v>32</v>
       </c>
@@ -6865,7 +6971,7 @@
       <c r="O61" s="25"/>
       <c r="P61" s="25"/>
     </row>
-    <row r="62" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" ht="14" customHeight="1">
       <c r="A62" s="13" t="s">
         <v>33</v>
       </c>
@@ -6887,7 +6993,7 @@
       <c r="O62" s="25"/>
       <c r="P62" s="25"/>
     </row>
-    <row r="63" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" ht="14" customHeight="1">
       <c r="A63" s="13" t="s">
         <v>34</v>
       </c>
@@ -6909,7 +7015,7 @@
       <c r="O63" s="25"/>
       <c r="P63" s="25"/>
     </row>
-    <row r="64" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" ht="14" customHeight="1">
       <c r="A64" s="13" t="s">
         <v>35</v>
       </c>
@@ -6929,7 +7035,7 @@
       <c r="O64" s="25"/>
       <c r="P64" s="25"/>
     </row>
-    <row r="65" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" ht="14" customHeight="1">
       <c r="A65" s="13"/>
       <c r="B65" s="25"/>
       <c r="C65" s="25"/>
@@ -6947,7 +7053,7 @@
       <c r="O65" s="25"/>
       <c r="P65" s="25"/>
     </row>
-    <row r="66" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" ht="14" customHeight="1">
       <c r="A66" s="13" t="s">
         <v>36</v>
       </c>
@@ -6969,7 +7075,7 @@
       <c r="O66" s="25"/>
       <c r="P66" s="25"/>
     </row>
-    <row r="67" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" ht="14" customHeight="1">
       <c r="A67" s="13" t="s">
         <v>36</v>
       </c>
@@ -6991,7 +7097,7 @@
       <c r="O67" s="25"/>
       <c r="P67" s="25"/>
     </row>
-    <row r="68" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" ht="14" customHeight="1">
       <c r="A68" s="13" t="s">
         <v>36</v>
       </c>
@@ -7013,7 +7119,7 @@
       <c r="O68" s="25"/>
       <c r="P68" s="25"/>
     </row>
-    <row r="69" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" ht="14" customHeight="1">
       <c r="A69" s="13" t="s">
         <v>36</v>
       </c>
@@ -7032,7 +7138,7 @@
       <c r="O69" s="25"/>
       <c r="P69" s="25"/>
     </row>
-    <row r="70" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" ht="14" customHeight="1">
       <c r="A70" s="13" t="s">
         <v>36</v>
       </c>
@@ -7051,7 +7157,7 @@
       <c r="O70" s="25"/>
       <c r="P70" s="25"/>
     </row>
-    <row r="71" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" ht="14" customHeight="1">
       <c r="A71" s="13" t="s">
         <v>37</v>
       </c>
@@ -7070,7 +7176,7 @@
       <c r="O71" s="25"/>
       <c r="P71" s="25"/>
     </row>
-    <row r="72" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" ht="14" customHeight="1">
       <c r="A72" s="13" t="s">
         <v>38</v>
       </c>
@@ -7090,7 +7196,7 @@
       <c r="O72" s="25"/>
       <c r="P72" s="25"/>
     </row>
-    <row r="73" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" ht="14" customHeight="1">
       <c r="A73" s="13" t="s">
         <v>38</v>
       </c>
@@ -7110,7 +7216,7 @@
       <c r="O73" s="25"/>
       <c r="P73" s="25"/>
     </row>
-    <row r="74" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" ht="14" customHeight="1">
       <c r="A74" s="31"/>
       <c r="B74" s="31"/>
       <c r="C74" s="31"/>
@@ -7128,7 +7234,7 @@
       <c r="O74" s="31"/>
       <c r="P74" s="31"/>
     </row>
-    <row r="75" spans="1:16" s="9" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" s="9" customFormat="1" ht="14" customHeight="1">
       <c r="A75" s="3" t="s">
         <v>39</v>
       </c>
@@ -7148,7 +7254,7 @@
       <c r="O75" s="7"/>
       <c r="P75" s="8"/>
     </row>
-    <row r="76" spans="1:16" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" s="12" customFormat="1" ht="14" customHeight="1">
       <c r="A76" s="10" t="s">
         <v>40</v>
       </c>
@@ -7168,7 +7274,7 @@
       <c r="O76" s="10"/>
       <c r="P76" s="11"/>
     </row>
-    <row r="77" spans="1:16" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" s="12" customFormat="1" ht="14" customHeight="1">
       <c r="A77" s="10" t="s">
         <v>41</v>
       </c>
@@ -7188,7 +7294,7 @@
       <c r="O77" s="10"/>
       <c r="P77" s="11"/>
     </row>
-    <row r="78" spans="1:16" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" s="12" customFormat="1" ht="14" customHeight="1">
       <c r="A78" s="10" t="s">
         <v>42</v>
       </c>
@@ -7208,7 +7314,7 @@
       <c r="O78" s="10"/>
       <c r="P78" s="11"/>
     </row>
-    <row r="79" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" ht="14" customHeight="1">
       <c r="A79" s="32" t="s">
         <v>43</v>
       </c>

</xml_diff>